<commit_message>
KIBON-2872 zahlungen statistik für institutionen + verbesserung authcheck für zahlungen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EFBD2E-1C65-4C2B-BC3C-2D19E8868068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FC3EA-6D77-4C5F-8018-1EA58884D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D62E91E4-9F0A-430C-8D32-ED35C134DAF2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D62E91E4-9F0A-430C-8D32-ED35C134DAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Zahlungen ausserhalb kiBon" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$N$1</definedName>
-    <definedName name="data">Data!$A$1:$Q$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$10:$N$10</definedName>
+    <definedName name="data">Data!$A$10:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="37" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>Titel Zahlungslauf</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Zeilenbeschriftungen</t>
   </si>
   <si>
-    <t>Ausbezahlt an Institutionen</t>
-  </si>
-  <si>
     <t>Zahlungen, die durch die Gemeinde ausserhalb von kiBon an die Antragstellenden gemacht werden müssen</t>
   </si>
   <si>
@@ -171,6 +168,36 @@
   </si>
   <si>
     <t>Ausserhalb kiBon</t>
+  </si>
+  <si>
+    <t>Summe Betreuungsgutscheine</t>
+  </si>
+  <si>
+    <t>Zahlungen ausserhalb kiBon</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>Zahlungen</t>
+  </si>
+  <si>
+    <t>Generiert am</t>
+  </si>
+  <si>
+    <t>{periodeParam}</t>
+  </si>
+  <si>
+    <t>{gemeindeParam}</t>
+  </si>
+  <si>
+    <t>{institutionParam}</t>
+  </si>
+  <si>
+    <t>{timestampParam}</t>
   </si>
 </sst>
 </file>
@@ -180,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +229,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +279,17 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6D9F1"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -252,10 +328,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,10 +380,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Neutral 2" xfId="2" xr:uid="{C8518E96-E25E-41E2-878D-3C6EB699AA47}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{0FAAEFE8-1E91-4F6E-AC75-76E5BE2784F3}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -327,9 +413,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Endtner Janik" refreshedDate="45042.752164814818" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{578D6903-A770-4468-8AF3-1F5119A8E80A}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Endtner Janik" refreshedDate="45043.463337615744" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{87B4536A-8A4B-4A6C-85CA-525487894EF0}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:Q1048576" sheet="Data"/>
+    <worksheetSource ref="A10:Q1048576" sheet="Data"/>
   </cacheSource>
   <cacheFields count="17">
     <cacheField name="Titel Zahlungslauf" numFmtId="0">
@@ -455,8 +541,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8A262662-859B-4891-858F-8DDE795858D1}" name="PivotTable1" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Ausbezahlt an Institutionen" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:C9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CC4BE9D-788D-443F-BDF3-AA5120CF541F}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe Betreuungsgutscheine" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:C10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
@@ -498,9 +584,9 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="4">
-        <item m="1" x="2"/>
         <item x="1"/>
         <item x="0"/>
+        <item m="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -531,7 +617,7 @@
   </colFields>
   <colItems count="2">
     <i>
-      <x v="2"/>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -556,7 +642,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16D9679E-396C-4D7A-9693-571F4361BBE6}" name="PivotTable1" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{134E440A-2B3E-4BA5-B82E-E57F1FF325CE}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
@@ -588,8 +674,8 @@
     <pivotField axis="axisPage" showAll="0">
       <items count="4">
         <item m="1" x="2"/>
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -621,11 +707,11 @@
     <i/>
   </colItems>
   <pageFields count="2">
-    <pageField fld="14" item="2" hier="-1"/>
     <pageField fld="1" item="0" hier="-1"/>
+    <pageField fld="14" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Summe von Betrag in CHF" fld="11" baseField="1" baseItem="0"/>
+    <dataField name="Zahlungen ausserhalb kiBon" fld="11" baseField="1" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -936,146 +1022,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D857DF-3A5E-41BF-BBE3-AE93EE84EC1F}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="30.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.88671875" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
-    <col min="9" max="10" width="19.44140625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="19.44140625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="21"/>
-    <col min="13" max="13" width="11.44140625" style="23"/>
-    <col min="14" max="14" width="18.88671875" style="23" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" style="23" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="21" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="23"/>
+    <col min="14" max="14" width="18.85546875" style="23" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" style="23" hidden="1" customWidth="1"/>
+    <col min="16" max="17" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="B11" s="7" t="str">
+        <f>IF(A11&lt;&gt;"","x","")</f>
+        <v>x</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="7" t="str">
-        <f>IF(A2&lt;&gt;"","x","")</f>
-        <v>x</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="I11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="L11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M11" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="N11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="O11" s="22" t="str">
+        <f>IF(N11="","Ausbezahlt an Institution","Ausserhalb kiBon")</f>
+        <v>Ausserhalb kiBon</v>
+      </c>
+      <c r="P11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="22" t="str">
-        <f>IF(N2="","Ausbezahlt an Institution","Ausserhalb kiBon")</f>
-        <v>Ausserhalb kiBon</v>
-      </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{48D857DF-3A5E-41BF-BBE3-AE93EE84EC1F}"/>
+  <autoFilter ref="A10:N10" xr:uid="{48D857DF-3A5E-41BF-BBE3-AE93EE84EC1F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:R2">
+  <conditionalFormatting sqref="A11:R11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$K2="X"</formula>
+      <formula>$K11="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1085,97 +1212,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D093B23D-6F3C-4F70-9C19-4A2F45F6DA0C}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0</v>
+      </c>
+      <c r="C7" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B8" s="30">
         <v>0</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C8" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="24">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="30">
         <v>0</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C9" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="24">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="30">
         <v>0</v>
       </c>
-      <c r="C8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="24">
-        <v>0</v>
-      </c>
-      <c r="C9" s="24">
+      <c r="C10" s="30">
         <v>0</v>
       </c>
     </row>
@@ -1189,76 +1317,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0A8E7A-1C75-4B38-9E99-490338CCC28D}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="24">
+        <v>21</v>
+      </c>
+      <c r="B7" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="24">
+        <v>33</v>
+      </c>
+      <c r="B8" s="30">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="24">
+        <v>12</v>
+      </c>
+      <c r="B9" s="30">
         <v>0</v>
       </c>
     </row>
@@ -1269,6 +1397,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D4B0DEBAADE082479C020A120548B899" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="96a75c11af173ed41e609e76c9db30b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad14f855-27c1-4510-b71d-42583984dc41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85ecfde502fbc4167fce567b17737251" ns2:_="">
     <xsd:import namespace="ad14f855-27c1-4510-b71d-42583984dc41"/>
@@ -1428,16 +1565,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F7F62F-D04B-4365-BA5A-CF4A7D48B356}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8C7096-A64B-4550-AA7F-CC742CB2CB00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1455,14 +1591,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F7F62F-D04B-4365-BA5A-CF4A7D48B356}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4a6500c8-aece-4f95-9ff4-aa2f25229e5c}" enabled="0" method="" siteId="{4a6500c8-aece-4f95-9ff4-aa2f25229e5c}" removed="1"/>

</xml_diff>

<commit_message>
KIBON-3022 ausgeblendete Spalten am Ende der Zahlungen Statistik platzieren, damit Text immer korrekt kopiert werden kann
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FC3EA-6D77-4C5F-8018-1EA58884D17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2FF1D7-C711-43A8-A41B-46C9D77B38B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D62E91E4-9F0A-430C-8D32-ED35C134DAF2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D62E91E4-9F0A-430C-8D32-ED35C134DAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Zahlungen ausserhalb kiBon" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$10:$N$10</definedName>
-    <definedName name="data">Data!$A$10:$Q$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$10:$M$10</definedName>
+    <definedName name="data">Data!$A$10:$O$11</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="71" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Endtner Janik" refreshedDate="45043.463337615744" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{87B4536A-8A4B-4A6C-85CA-525487894EF0}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Endtner Janik" refreshedDate="45131.452174999999" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{B4A3DE99-FA8B-4948-95CB-A6C8D4F367FC}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A10:Q1048576" sheet="Data"/>
   </cacheSource>
@@ -421,72 +421,71 @@
     <cacheField name="Titel Zahlungslauf" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
+    <cacheField name="Gemeinde" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="{gemeinde}"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Institution" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="{institution}"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Erstellungsdatum Zahlungslauf" numFmtId="22">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Kind Nachname" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Kind Vorname" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Referenznummer" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="{referenznummer}"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="von" numFmtId="14">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="bis" numFmtId="14">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="BG-Pensum" numFmtId="10">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Betrag in CHF" numFmtId="164">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Korrektur" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="In Zahlungslauf ignorieren" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="IBAN Eltern" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="{ibanEltern}"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Kontoname Eltern" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
     <cacheField name="Nicht leer" numFmtId="0">
       <sharedItems containsBlank="1" count="2">
         <s v="x"/>
         <m/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Gemeinde" numFmtId="0">
+    <cacheField name="Auszahlung an" numFmtId="0">
       <sharedItems containsBlank="1" count="2">
-        <s v="{gemeinde}"/>
+        <s v="Ausserhalb kiBon"/>
         <m/>
       </sharedItems>
-    </cacheField>
-    <cacheField name="Institution" numFmtId="0">
-      <sharedItems containsBlank="1" count="2">
-        <s v="{institution}"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Erstellungsdatum Zahlungslauf" numFmtId="22">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Kind Nachname" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Kind Vorname" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Referenznummer" numFmtId="0">
-      <sharedItems containsBlank="1" count="2">
-        <s v="{referenznummer}"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="von" numFmtId="14">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="bis" numFmtId="14">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="BG-Pensum" numFmtId="10">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Betrag in CHF" numFmtId="164">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Korrektur" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="In Zahlungslauf ignorieren" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Auszahlung an" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="Ausserhalb kiBon"/>
-        <m/>
-        <s v="Ausbezahlt an Institution" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="IBAN Eltern" numFmtId="0">
-      <sharedItems containsBlank="1" count="2">
-        <s v="{ibanEltern}"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Kontoname Eltern" numFmtId="0">
-      <sharedItems containsBlank="1"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -503,7 +502,6 @@
     <s v="{zahlungslaufTitle}"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
     <s v="{timestampZahlungslauf}"/>
     <s v="{kindNachname}"/>
     <s v="{kindVorname}"/>
@@ -515,12 +513,12 @@
     <s v="{korrektur}"/>
     <s v="{ignorieren}"/>
     <x v="0"/>
+    <s v="{kontoEltern}"/>
     <x v="0"/>
-    <s v="{kontoEltern}"/>
+    <x v="0"/>
   </r>
   <r>
     <m/>
-    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <m/>
@@ -534,24 +532,18 @@
     <m/>
     <m/>
     <x v="1"/>
+    <m/>
     <x v="1"/>
-    <m/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3CC4BE9D-788D-443F-BDF3-AA5120CF541F}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe Betreuungsgutscheine" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4267A76C-AEEE-49A0-BD78-BF3E886C4F6C}" name="PivotTable1" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe Betreuungsgutscheine" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="0"/>
@@ -582,21 +574,27 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
-        <item m="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="ascending">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
   <rowFields count="3">
+    <field x="1"/>
     <field x="2"/>
-    <field x="3"/>
-    <field x="7"/>
+    <field x="6"/>
   </rowFields>
   <rowItems count="4">
     <i>
@@ -613,21 +611,21 @@
     </i>
   </rowItems>
   <colFields count="1">
-    <field x="14"/>
+    <field x="16"/>
   </colFields>
   <colItems count="2">
     <i>
-      <x v="1"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="1" item="0" hier="-1"/>
+    <pageField fld="15" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Summe von Betrag in CHF" fld="11" baseField="1" baseItem="0"/>
+    <dataField name="Summe von Betrag in CHF" fld="10" baseField="1" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -642,10 +640,36 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{134E440A-2B3E-4BA5-B82E-E57F1FF325CE}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4F05E15A-369D-4E77-9BF2-D2D4865EE276}" name="PivotTable1" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Summe" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="3">
         <item x="0"/>
@@ -653,44 +677,17 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisPage" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item m="1" x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="2">
-    <field x="2"/>
-    <field x="15"/>
+    <field x="1"/>
+    <field x="13"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -707,11 +704,11 @@
     <i/>
   </colItems>
   <pageFields count="2">
-    <pageField fld="1" item="0" hier="-1"/>
-    <pageField fld="14" item="1" hier="-1"/>
+    <pageField fld="15" item="0" hier="-1"/>
+    <pageField fld="16" item="0" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Zahlungen ausserhalb kiBon" fld="11" baseField="1" baseItem="0"/>
+    <dataField name="Zahlungen ausserhalb kiBon" fld="10" baseField="1" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1026,183 +1023,182 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="10" width="19.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="21" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="23"/>
-    <col min="14" max="14" width="18.85546875" style="23" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="23" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="23.28515625" customWidth="1"/>
+    <col min="1" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="30.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="9" width="19.44140625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="23"/>
+    <col min="13" max="13" width="18.88671875" style="23" customWidth="1"/>
+    <col min="14" max="15" width="23.33203125" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" style="23" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="25"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="B6" s="27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="B7" s="29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="8" t="s">
+      <c r="Q10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="7" t="str">
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" s="7" t="str">
         <f>IF(A11&lt;&gt;"","x","")</f>
         <v>x</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="22" t="str">
-        <f>IF(N11="","Ausbezahlt an Institution","Ausserhalb kiBon")</f>
+      <c r="Q11" s="22" t="str">
+        <f>IF(M11="","Ausbezahlt an Institution","Ausserhalb kiBon")</f>
         <v>Ausserhalb kiBon</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A10:N10" xr:uid="{48D857DF-3A5E-41BF-BBE3-AE93EE84EC1F}"/>
+  <autoFilter ref="A10:M10" xr:uid="{48D857DF-3A5E-41BF-BBE3-AE93EE84EC1F}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A11:R11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$K11="X"</formula>
+      <formula>$J11="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1215,27 +1211,27 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1243,8 +1239,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1285,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>41</v>
       </c>
@@ -1318,30 +1314,30 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+      <selection activeCell="A5" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1349,7 +1345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1357,8 +1353,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1366,7 +1362,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1374,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1382,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1397,15 +1393,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D4B0DEBAADE082479C020A120548B899" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="96a75c11af173ed41e609e76c9db30b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ad14f855-27c1-4510-b71d-42583984dc41" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85ecfde502fbc4167fce567b17737251" ns2:_="">
     <xsd:import namespace="ad14f855-27c1-4510-b71d-42583984dc41"/>
@@ -1565,15 +1552,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F7F62F-D04B-4365-BA5A-CF4A7D48B356}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F8C7096-A64B-4550-AA7F-CC742CB2CB00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1591,6 +1579,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3F7F62F-D04B-4365-BA5A-CF4A7D48B356}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4a6500c8-aece-4f95-9ff4-aa2f25229e5c}" enabled="0" method="" siteId="{4a6500c8-aece-4f95-9ff4-aa2f25229e5c}" removed="1"/>

</xml_diff>

<commit_message>
KIBON-3044 Anpassung Zahlungen Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Zahlungen_DE.xlsx
@@ -163,13 +163,13 @@
     <t xml:space="preserve">Auszahlungen an Institution</t>
   </si>
   <si>
+    <t xml:space="preserve">- all -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summe von Betrag in CHF</t>
+  </si>
+  <si>
     <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summe von Betrag in CHF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ausserhalb kiBon</t>
   </si>
   <si>
     <t xml:space="preserve">Total Result</t>
@@ -187,8 +187,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="&quot;CHF &quot;#,##0.00"/>
   </numFmts>
@@ -498,27 +498,27 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="58">
@@ -550,15 +550,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,131 +626,131 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="26" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="26" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="25" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="27" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="26" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -763,13 +763,13 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Neutral 2" xfId="20"/>
-    <cellStyle name="Standard 2" xfId="21"/>
-    <cellStyle name="Pivot Table Field" xfId="22"/>
-    <cellStyle name="Pivot Table Corner" xfId="23"/>
-    <cellStyle name="Pivot Table Value" xfId="24"/>
-    <cellStyle name="Pivot Table Category" xfId="25"/>
-    <cellStyle name="Pivot Table Title" xfId="26"/>
-    <cellStyle name="Pivot Table Result" xfId="27"/>
+    <cellStyle name="Pivot Table Category" xfId="21"/>
+    <cellStyle name="Pivot Table Corner" xfId="22"/>
+    <cellStyle name="Pivot Table Field" xfId="23"/>
+    <cellStyle name="Pivot Table Result" xfId="24"/>
+    <cellStyle name="Pivot Table Title" xfId="25"/>
+    <cellStyle name="Pivot Table Value" xfId="26"/>
+    <cellStyle name="Standard 2" xfId="27"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -865,10 +865,16 @@
   <cacheSource type="worksheet">
     <worksheetSource ref="A10:R1048576" sheet="Data"/>
   </cacheSource>
-  <cacheFields count="17">
+  <cacheFields count="18">
     <cacheField name="Titel Zahlungslauf" numFmtId="0">
       <sharedItems containsBlank="1" count="2">
         <s v="{zahlungslaufTitle}"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Fälligkeitsdatum" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="{faelligkeitsDatum}"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -992,6 +998,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
+    <x v="0"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -999,7 +1006,7 @@
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1" compact="0" compactData="0">
   <location ref="A5:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="17">
+  <pivotFields count="18">
     <pivotField compact="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0">
       <items count="3">
@@ -1036,17 +1043,18 @@
     <pivotField axis="axisPage" compact="0" showAll="0">
       <items count="3">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" compact="0" showAll="0">
       <items count="3">
         <item x="0"/>
-        <item x="1"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" showAll="0"/>
   </pivotFields>
   <rowFields count="3">
     <field x="1"/>
@@ -1069,7 +1077,7 @@
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1" compact="0" compactData="0">
   <location ref="A6:C9" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="2" colPageCount="1"/>
-  <pivotFields count="17">
+  <pivotFields count="18">
     <pivotField compact="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0">
       <items count="3">
@@ -1100,7 +1108,7 @@
     <pivotField axis="axisPage" compact="0" showAll="0">
       <items count="3">
         <item x="0"/>
-        <item h="1" x="1"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1111,6 +1119,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" showAll="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="1"/>
@@ -1135,16 +1144,18 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.45703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="16.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="5" width="11.44"/>
@@ -1154,24 +1165,24 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="5" width="18.89"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="Q3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="Q3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1179,7 +1190,7 @@
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1187,7 +1198,7 @@
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1199,11 +1210,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" s="17" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="17" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1212,7 +1223,7 @@
       <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="11" t="s">
@@ -1224,10 +1235,10 @@
       <c r="H10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="14" t="s">
@@ -1259,7 +1270,7 @@
       <c r="A11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1268,7 +1279,7 @@
       <c r="D11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="18" t="s">
@@ -1280,10 +1291,10 @@
       <c r="H11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="21" t="s">
@@ -1342,10 +1353,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.45703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.33"/>
@@ -1364,7 +1375,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>44</v>
@@ -1378,19 +1389,19 @@
       <c r="B5" s="28"/>
       <c r="C5" s="29"/>
       <c r="D5" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>6</v>
-      </c>
       <c r="C6" s="33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>46</v>
@@ -1401,7 +1412,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="38"/>
@@ -1411,7 +1422,7 @@
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="41"/>
       <c r="B8" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="43"/>
@@ -1421,7 +1432,7 @@
       <c r="A9" s="45"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="47"/>
       <c r="E9" s="48"/>
@@ -1454,10 +1465,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="B:B A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.45703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.78"/>
@@ -1475,11 +1486,11 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>44</v>
@@ -1487,7 +1498,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>46</v>
@@ -1496,10 +1507,10 @@
     <row r="5" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="54" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>49</v>
@@ -1507,7 +1518,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="42"/>
       <c r="C7" s="56"/>
@@ -1515,7 +1526,7 @@
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="45"/>
       <c r="B8" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="57"/>
     </row>

</xml_diff>